<commit_message>
comparing 2-pt total attempts to 3-pt total attempts within a 24-year period - complete
</commit_message>
<xml_diff>
--- a/team_totals_three_point_field_goals_2001_to_2024_pivot_table.xlsx
+++ b/team_totals_three_point_field_goals_2001_to_2024_pivot_table.xlsx
@@ -14,9 +14,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>season_ending_year</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
   <si>
     <t>Atlanta Hawks</t>
@@ -492,82 +564,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>2001</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2002</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2003</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2004</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2005</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2006</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2007</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2008</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2009</v>
-      </c>
-      <c r="K1" s="1">
-        <v>2010</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2011</v>
-      </c>
-      <c r="M1" s="1">
-        <v>2012</v>
-      </c>
-      <c r="N1" s="1">
-        <v>2013</v>
-      </c>
-      <c r="O1" s="1">
-        <v>2014</v>
-      </c>
-      <c r="P1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="R1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="S1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="T1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="U1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="V1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="W1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="X1" s="1">
-        <v>2023</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>2024</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>333</v>
@@ -644,7 +716,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>592</v>
@@ -721,7 +793,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="N4">
         <v>628</v>
@@ -762,7 +834,7 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F5">
         <v>320</v>
@@ -797,7 +869,7 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>340</v>
@@ -838,7 +910,7 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>329</v>
@@ -915,7 +987,7 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>220</v>
@@ -992,7 +1064,7 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>517</v>
@@ -1069,7 +1141,7 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>512</v>
@@ -1146,7 +1218,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>389</v>
@@ -1223,7 +1295,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>282</v>
@@ -1300,7 +1372,7 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>504</v>
@@ -1377,7 +1449,7 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>396</v>
@@ -1454,7 +1526,7 @@
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>360</v>
@@ -1531,7 +1603,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>439</v>
@@ -1608,7 +1680,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>336</v>
@@ -1682,7 +1754,7 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>478</v>
@@ -1759,7 +1831,7 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>562</v>
@@ -1836,7 +1908,7 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>322</v>
@@ -1913,7 +1985,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B21">
         <v>361</v>
@@ -1954,7 +2026,7 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D22">
         <v>404</v>
@@ -1986,7 +2058,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="O23">
         <v>486</v>
@@ -2024,7 +2096,7 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="G24">
         <v>300</v>
@@ -2035,7 +2107,7 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <v>391</v>
@@ -2112,7 +2184,7 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="J26">
         <v>328</v>
@@ -2165,7 +2237,7 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>490</v>
@@ -2242,7 +2314,7 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B28">
         <v>262</v>
@@ -2319,7 +2391,7 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B29">
         <v>332</v>
@@ -2396,7 +2468,7 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B30">
         <v>369</v>
@@ -2473,7 +2545,7 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B31">
         <v>479</v>
@@ -2550,7 +2622,7 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B32">
         <v>445</v>
@@ -2627,7 +2699,7 @@
     </row>
     <row r="33" spans="1:25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B33">
         <v>466</v>
@@ -2656,7 +2728,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B34">
         <v>429</v>
@@ -2733,7 +2805,7 @@
     </row>
     <row r="35" spans="1:25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B35">
         <v>325</v>
@@ -2810,7 +2882,7 @@
     </row>
     <row r="36" spans="1:25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B36">
         <v>325</v>
@@ -2818,7 +2890,7 @@
     </row>
     <row r="37" spans="1:25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B37">
         <v>275</v>

</xml_diff>

<commit_message>
manipulating team data - in progress
</commit_message>
<xml_diff>
--- a/team_totals_three_point_field_goals_2001_to_2024_pivot_table.xlsx
+++ b/team_totals_three_point_field_goals_2001_to_2024_pivot_table.xlsx
@@ -14,81 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>season_ending_year</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
-    <t>2002</t>
-  </si>
-  <si>
-    <t>2003</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>2006</t>
-  </si>
-  <si>
-    <t>2007</t>
-  </si>
-  <si>
-    <t>2008</t>
-  </si>
-  <si>
-    <t>2009</t>
-  </si>
-  <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>2024</t>
   </si>
   <si>
     <t>Atlanta Hawks</t>
@@ -564,82 +492,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
+      <c r="B1" s="1">
+        <v>2001</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2004</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2005</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2007</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2008</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2024</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>333</v>
@@ -716,7 +644,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>592</v>
@@ -793,7 +721,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="N4">
         <v>628</v>
@@ -834,7 +762,7 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>320</v>
@@ -869,7 +797,7 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>340</v>
@@ -910,7 +838,7 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>329</v>
@@ -987,7 +915,7 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>220</v>
@@ -1064,7 +992,7 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>517</v>
@@ -1141,7 +1069,7 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>512</v>
@@ -1218,7 +1146,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>389</v>
@@ -1295,7 +1223,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>282</v>
@@ -1372,7 +1300,7 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>504</v>
@@ -1449,7 +1377,7 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>396</v>
@@ -1526,7 +1454,7 @@
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>360</v>
@@ -1603,7 +1531,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>439</v>
@@ -1680,7 +1608,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>336</v>
@@ -1754,7 +1682,7 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>478</v>
@@ -1831,7 +1759,7 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>562</v>
@@ -1908,7 +1836,7 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>322</v>
@@ -1985,7 +1913,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>361</v>
@@ -2026,7 +1954,7 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D22">
         <v>404</v>
@@ -2058,7 +1986,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="O23">
         <v>486</v>
@@ -2096,7 +2024,7 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G24">
         <v>300</v>
@@ -2107,7 +2035,7 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>391</v>
@@ -2184,7 +2112,7 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="J26">
         <v>328</v>
@@ -2237,7 +2165,7 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>490</v>
@@ -2314,7 +2242,7 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>262</v>
@@ -2391,7 +2319,7 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>332</v>
@@ -2468,7 +2396,7 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>369</v>
@@ -2545,7 +2473,7 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>479</v>
@@ -2622,7 +2550,7 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>445</v>
@@ -2699,7 +2627,7 @@
     </row>
     <row r="33" spans="1:25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>466</v>
@@ -2728,7 +2656,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>429</v>
@@ -2805,7 +2733,7 @@
     </row>
     <row r="35" spans="1:25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>325</v>
@@ -2882,7 +2810,7 @@
     </row>
     <row r="36" spans="1:25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>325</v>
@@ -2890,7 +2818,7 @@
     </row>
     <row r="37" spans="1:25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>275</v>

</xml_diff>